<commit_message>
reuqirement traceability matrix - Khang 08/12
</commit_message>
<xml_diff>
--- a/3. Requirement/AS_RE_RequirementTraceabilityMatrix.xlsx
+++ b/3. Requirement/AS_RE_RequirementTraceabilityMatrix.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Requirement_Traceability_Matrix!$A$5:$G$26</definedName>
   </definedNames>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -398,9 +398,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -423,6 +420,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -763,7 +763,7 @@
   <dimension ref="A1:G43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,580 +1283,580 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="17"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="25"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:7" s="2" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="19" t="s">
+      <c r="G5" s="18" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21" t="s">
+      <c r="C6" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" s="19"/>
+      <c r="E6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G6" s="24" t="s">
+      <c r="F6" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="A7" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="21" t="s">
+      <c r="B7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21" t="s">
+      <c r="C7" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="19"/>
+      <c r="E7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G7" s="24" t="s">
+      <c r="F7" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="A8" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21" t="s">
+      <c r="C8" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="19"/>
+      <c r="E8" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G8" s="24" t="s">
+      <c r="F8" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G8" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="A9" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="21" t="s">
+      <c r="B9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21" t="s">
+      <c r="C9" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="24" t="s">
+      <c r="F9" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="21" t="s">
+      <c r="C10" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" s="19"/>
+      <c r="E10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G10" s="24" t="s">
+      <c r="F10" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G10" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="21" t="s">
+      <c r="B11" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D11" s="20"/>
-      <c r="E11" s="21" t="s">
+      <c r="C11" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="19"/>
+      <c r="E11" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G11" s="24" t="s">
+      <c r="F11" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="21" t="s">
+      <c r="B12" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="20"/>
-      <c r="E12" s="21" t="s">
+      <c r="C12" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="19"/>
+      <c r="E12" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="24" t="s">
+      <c r="F12" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="20" t="s">
+      <c r="A13" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="20"/>
-      <c r="E13" s="21" t="s">
+      <c r="C13" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" s="19"/>
+      <c r="E13" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G13" s="24" t="s">
+      <c r="F13" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G13" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+      <c r="A14" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D14" s="20"/>
-      <c r="E14" s="21" t="s">
+      <c r="C14" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D14" s="19"/>
+      <c r="E14" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" s="24" t="s">
+      <c r="F14" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G14" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
+      <c r="A15" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="21" t="s">
+      <c r="B15" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="C15" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D15" s="20"/>
-      <c r="E15" s="21" t="s">
+      <c r="C15" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="19"/>
+      <c r="E15" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G15" s="24" t="s">
+      <c r="F15" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G15" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21" t="s">
+      <c r="C16" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D16" s="19"/>
+      <c r="E16" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G16" s="24" t="s">
+      <c r="F16" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="21" t="s">
+      <c r="C17" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="19"/>
+      <c r="E17" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G17" s="24" t="s">
+      <c r="F17" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G17" s="23" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="21" t="s">
+      <c r="C18" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="19"/>
+      <c r="E18" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18" s="24" t="s">
+      <c r="F18" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G18" s="23" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="20" t="s">
+      <c r="A19" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="21" t="s">
+      <c r="B19" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="20"/>
-      <c r="E19" s="21" t="s">
+      <c r="C19" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" s="19"/>
+      <c r="E19" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="24" t="s">
+      <c r="F19" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="23" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="C20" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="20"/>
-      <c r="E20" s="21" t="s">
+      <c r="C20" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" s="19"/>
+      <c r="E20" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="F20" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="24" t="s">
+      <c r="F20" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G20" s="23" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
+      <c r="A21" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D21" s="20"/>
-      <c r="E21" s="21" t="s">
+      <c r="C21" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" s="19"/>
+      <c r="E21" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21" s="24" t="s">
+      <c r="F21" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G21" s="23" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
+      <c r="A22" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="21" t="s">
+      <c r="B22" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="21" t="s">
+      <c r="C22" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" s="19"/>
+      <c r="E22" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G22" s="24" t="s">
+      <c r="F22" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G22" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B23" s="21" t="s">
+      <c r="B23" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C23" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="20"/>
-      <c r="E23" s="21" t="s">
+      <c r="C23" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="19"/>
+      <c r="E23" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G23" s="24" t="s">
+      <c r="F23" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G23" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="21" t="s">
+      <c r="B24" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="21" t="s">
+      <c r="C24" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D24" s="19"/>
+      <c r="E24" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G24" s="24" t="s">
+      <c r="F24" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G24" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" s="20"/>
-      <c r="E25" s="21" t="s">
+      <c r="C25" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="19"/>
+      <c r="E25" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G25" s="24" t="s">
+      <c r="F25" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G25" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="21" t="s">
+      <c r="B26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="21" t="s">
+      <c r="C26" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="19"/>
+      <c r="E26" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G26" s="24" t="s">
+      <c r="F26" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G26" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D27" s="25"/>
-      <c r="E27" s="21" t="s">
+      <c r="C27" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" s="24"/>
+      <c r="E27" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F27" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G27" s="24" t="s">
+      <c r="F27" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G27" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="21" t="s">
+      <c r="B28" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C28" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D28" s="25"/>
-      <c r="E28" s="21" t="s">
+      <c r="C28" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D28" s="24"/>
+      <c r="E28" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="F28" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G28" s="24" t="s">
+      <c r="F28" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G28" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="21" t="s">
+      <c r="B29" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C29" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D29" s="25"/>
-      <c r="E29" s="21" t="s">
+      <c r="C29" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D29" s="24"/>
+      <c r="E29" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="F29" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G29" s="24" t="s">
+      <c r="F29" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G29" s="23" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="25"/>
-      <c r="E30" s="21" t="s">
+      <c r="C30" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D30" s="24"/>
+      <c r="E30" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="F30" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="G30" s="24" t="s">
+      <c r="F30" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G30" s="23" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>